<commit_message>
fixed error in ajouter_eng (avenant)
</commit_message>
<xml_diff>
--- a/anydesk.xlsx
+++ b/anydesk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>Direction</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>10,7,0,253</t>
+  </si>
+  <si>
+    <t>last update</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>fixed error in ajouter_eng (avenant)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +231,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD28"/>
+  <dimension ref="A1:BF28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -519,13 +531,14 @@
     <col min="6" max="6" width="17.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="8" customWidth="1"/>
-    <col min="11" max="56" width="9.140625" style="8"/>
-    <col min="57" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="10" width="14.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="8" customWidth="1"/>
+    <col min="13" max="58" width="9.140625" style="8"/>
+    <col min="59" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -553,11 +566,15 @@
       <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -602,8 +619,10 @@
       <c r="BB1" s="8"/>
       <c r="BC1" s="8"/>
       <c r="BD1" s="8"/>
-    </row>
-    <row r="2" spans="1:56" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+    </row>
+    <row r="2" spans="1:58" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -629,11 +648,11 @@
         <v>24</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -678,8 +697,10 @@
       <c r="BB2" s="8"/>
       <c r="BC2" s="8"/>
       <c r="BD2" s="8"/>
-    </row>
-    <row r="3" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+    </row>
+    <row r="3" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -705,9 +726,8 @@
       <c r="I3" s="10">
         <v>45596</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -752,8 +772,10 @@
       <c r="BB3" s="8"/>
       <c r="BC3" s="8"/>
       <c r="BD3" s="8"/>
-    </row>
-    <row r="4" spans="1:56" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+    </row>
+    <row r="4" spans="1:58" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -781,9 +803,8 @@
       <c r="I4" s="10">
         <v>45596</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
@@ -828,8 +849,10 @@
       <c r="BB4" s="8"/>
       <c r="BC4" s="8"/>
       <c r="BD4" s="8"/>
-    </row>
-    <row r="5" spans="1:56" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+    </row>
+    <row r="5" spans="1:58" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -857,11 +880,11 @@
       <c r="I5" s="10">
         <v>45596</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -906,8 +929,10 @@
       <c r="BB5" s="8"/>
       <c r="BC5" s="8"/>
       <c r="BD5" s="8"/>
-    </row>
-    <row r="6" spans="1:56" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="BE5" s="8"/>
+      <c r="BF5" s="8"/>
+    </row>
+    <row r="6" spans="1:58" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -935,11 +960,11 @@
       <c r="I6" s="10">
         <v>45596</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
@@ -984,8 +1009,10 @@
       <c r="BB6" s="8"/>
       <c r="BC6" s="8"/>
       <c r="BD6" s="8"/>
-    </row>
-    <row r="7" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE6" s="8"/>
+      <c r="BF6" s="8"/>
+    </row>
+    <row r="7" spans="1:58" s="3" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1013,9 +1040,12 @@
       <c r="I7" s="10">
         <v>45596</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="J7" s="10">
+        <v>45377</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -1060,8 +1090,10 @@
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
       <c r="BD7" s="8"/>
-    </row>
-    <row r="8" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="8"/>
+    </row>
+    <row r="8" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1087,11 +1119,11 @@
       <c r="I8" s="10">
         <v>45596</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -1136,8 +1168,10 @@
       <c r="BB8" s="8"/>
       <c r="BC8" s="8"/>
       <c r="BD8" s="8"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="BE8" s="8"/>
+      <c r="BF8" s="8"/>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1163,11 +1197,13 @@
       <c r="I9" s="10">
         <v>45596</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:56" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" s="3" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1195,11 +1231,11 @@
       <c r="I10" s="10">
         <v>45596</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1244,8 +1280,10 @@
       <c r="BB10" s="8"/>
       <c r="BC10" s="8"/>
       <c r="BD10" s="8"/>
-    </row>
-    <row r="11" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BE10" s="8"/>
+      <c r="BF10" s="8"/>
+    </row>
+    <row r="11" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1268,11 +1306,13 @@
         <v>19</v>
       </c>
       <c r="I11" s="10">
-        <v>45597</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+        <v>45566</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -1317,19 +1357,42 @@
       <c r="BB11" s="8"/>
       <c r="BC11" s="8"/>
       <c r="BD11" s="8"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="BE11" s="8"/>
+      <c r="BF11" s="8"/>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1565013331</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="10">
+        <v>45566</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1339,8 +1402,11 @@
       <c r="G13" s="3"/>
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1350,8 +1416,11 @@
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1361,8 +1430,11 @@
       <c r="G15" s="3"/>
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1372,8 +1444,11 @@
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1383,8 +1458,11 @@
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1394,8 +1472,11 @@
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1405,8 +1486,11 @@
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1416,8 +1500,11 @@
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1427,8 +1514,11 @@
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1438,8 +1528,11 @@
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1449,8 +1542,11 @@
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1460,8 +1556,11 @@
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1471,8 +1570,11 @@
       <c r="G25" s="3"/>
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1482,8 +1584,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1493,8 +1598,11 @@
       <c r="G27" s="3"/>
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1504,6 +1612,9 @@
       <c r="G28" s="3"/>
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mila payment (part 1)
</commit_message>
<xml_diff>
--- a/anydesk.xlsx
+++ b/anydesk.xlsx
@@ -652,7 +652,7 @@
   <dimension ref="A1:BF28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,7 @@
         <v>234009317</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>16</v>
@@ -1361,10 +1361,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="3">
-        <v>1590730343</v>
+        <v>1085627854</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>16</v>
@@ -1378,7 +1378,9 @@
       <c r="I10" s="9">
         <v>45596</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9">
+        <v>45501</v>
+      </c>
       <c r="K10" s="10"/>
       <c r="L10" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
dep in guezzam among oder tings
</commit_message>
<xml_diff>
--- a/anydesk.xlsx
+++ b/anydesk.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="65">
   <si>
     <t>Direction</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>31/11/2025</t>
+  </si>
+  <si>
+    <t>port 8090 for phpmyadmin</t>
   </si>
 </sst>
 </file>
@@ -704,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1947,10 +1950,10 @@
         <v>59</v>
       </c>
       <c r="D22" s="3">
-        <v>1356948900</v>
+        <v>1640258972</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>16</v>
@@ -2125,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2144,7 +2147,8 @@
     <col min="12" max="12" width="21.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="16.140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="19" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2272,7 +2276,9 @@
       <c r="N2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>

</xml_diff>